<commit_message>
ready to do contingencies
</commit_message>
<xml_diff>
--- a/Code/Results/res_bus/vm_pu.xlsx
+++ b/Code/Results/res_bus/vm_pu.xlsx
@@ -421,34 +421,34 @@
         <v>1.05</v>
       </c>
       <c r="C2">
-        <v>0.9584483529348087</v>
+        <v>0.9584483529348066</v>
       </c>
       <c r="D2">
-        <v>0.9855021302359518</v>
+        <v>0.9855021302359501</v>
       </c>
       <c r="E2">
-        <v>0.9674641479476159</v>
+        <v>0.9674641479476135</v>
       </c>
       <c r="F2">
-        <v>0.9293225045445663</v>
+        <v>0.9293225045445632</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1.030311226548108</v>
+        <v>1.030311226548107</v>
       </c>
       <c r="J2">
-        <v>0.9819471009265013</v>
+        <v>0.9819471009264992</v>
       </c>
       <c r="K2">
-        <v>0.9971672080651706</v>
+        <v>0.9971672080651687</v>
       </c>
       <c r="L2">
-        <v>0.9793961721171767</v>
+        <v>0.9793961721171743</v>
       </c>
       <c r="M2">
-        <v>0.9418629691489703</v>
+        <v>0.9418629691489674</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -459,34 +459,34 @@
         <v>1.05</v>
       </c>
       <c r="C3">
-        <v>0.9706497244047197</v>
+        <v>0.9706497244047185</v>
       </c>
       <c r="D3">
-        <v>0.9949150197488773</v>
+        <v>0.9949150197488759</v>
       </c>
       <c r="E3">
-        <v>0.9780820343366293</v>
+        <v>0.9780820343366284</v>
       </c>
       <c r="F3">
-        <v>0.9452002625583125</v>
+        <v>0.9452002625583111</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1.034465343064478</v>
+        <v>1.034465343064477</v>
       </c>
       <c r="J3">
-        <v>0.9919737936820995</v>
+        <v>0.9919737936820984</v>
       </c>
       <c r="K3">
-        <v>1.005613379990295</v>
+        <v>1.005613379990294</v>
       </c>
       <c r="L3">
-        <v>0.9890032599271316</v>
+        <v>0.9890032599271307</v>
       </c>
       <c r="M3">
-        <v>0.9565859002114416</v>
+        <v>0.9565859002114402</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -500,13 +500,13 @@
         <v>0.9781351793452007</v>
       </c>
       <c r="D4">
-        <v>1.000693896848053</v>
+        <v>1.000693896848054</v>
       </c>
       <c r="E4">
-        <v>0.9845980165487557</v>
+        <v>0.9845980165487556</v>
       </c>
       <c r="F4">
-        <v>0.9549201151871431</v>
+        <v>0.9549201151871438</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -515,16 +515,16 @@
         <v>1.036992108816931</v>
       </c>
       <c r="J4">
-        <v>0.9981152228703128</v>
+        <v>0.9981152228703127</v>
       </c>
       <c r="K4">
         <v>1.010783954354648</v>
       </c>
       <c r="L4">
-        <v>0.9948859544474211</v>
+        <v>0.994885954447421</v>
       </c>
       <c r="M4">
-        <v>0.9655948894583619</v>
+        <v>0.9655948894583626</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -535,16 +535,16 @@
         <v>1.05</v>
       </c>
       <c r="C5">
-        <v>0.9811938147937375</v>
+        <v>0.9811938147937374</v>
       </c>
       <c r="D5">
         <v>1.003055903250167</v>
       </c>
       <c r="E5">
-        <v>0.987260819687118</v>
+        <v>0.9872608196871177</v>
       </c>
       <c r="F5">
-        <v>0.9588879826722939</v>
+        <v>0.9588879826722936</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -559,10 +559,10 @@
         <v>1.012893907439006</v>
       </c>
       <c r="L5">
-        <v>0.9972869374221054</v>
+        <v>0.9972869374221052</v>
       </c>
       <c r="M5">
-        <v>0.9692714908538137</v>
+        <v>0.9692714908538133</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -573,34 +573,34 @@
         <v>1.05</v>
       </c>
       <c r="C6">
-        <v>0.9817024533519729</v>
+        <v>0.9817024533519719</v>
       </c>
       <c r="D6">
-        <v>1.003448728361516</v>
+        <v>1.003448728361515</v>
       </c>
       <c r="E6">
-        <v>0.9877036463588168</v>
+        <v>0.9877036463588158</v>
       </c>
       <c r="F6">
-        <v>0.9595476339635669</v>
+        <v>0.9595476339635655</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1.038189758197654</v>
+        <v>1.038189758197653</v>
       </c>
       <c r="J6">
-        <v>1.001039042129263</v>
+        <v>1.001039042129262</v>
       </c>
       <c r="K6">
-        <v>1.013244615583668</v>
+        <v>1.013244615583667</v>
       </c>
       <c r="L6">
-        <v>0.997686047603373</v>
+        <v>0.997686047603372</v>
       </c>
       <c r="M6">
-        <v>0.9698826528835146</v>
+        <v>0.9698826528835135</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -614,13 +614,13 @@
         <v>0.9781763839838064</v>
       </c>
       <c r="D7">
-        <v>1.000725714391077</v>
+        <v>1.000725714391078</v>
       </c>
       <c r="E7">
-        <v>0.9846338877011357</v>
+        <v>0.9846338877011361</v>
       </c>
       <c r="F7">
-        <v>0.9549735820594123</v>
+        <v>0.9549735820594124</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -629,16 +629,16 @@
         <v>1.037005967410858</v>
       </c>
       <c r="J7">
-        <v>0.9981490063742641</v>
+        <v>0.9981490063742642</v>
       </c>
       <c r="K7">
         <v>1.010812390040263</v>
       </c>
       <c r="L7">
-        <v>0.9949183104728457</v>
+        <v>0.9949183104728458</v>
       </c>
       <c r="M7">
-        <v>0.9656444359673054</v>
+        <v>0.9656444359673056</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -649,16 +649,16 @@
         <v>1.05</v>
       </c>
       <c r="C8">
-        <v>0.9626631606695668</v>
+        <v>0.9626631606695669</v>
       </c>
       <c r="D8">
-        <v>0.9887526067434366</v>
+        <v>0.9887526067434367</v>
       </c>
       <c r="E8">
-        <v>0.9711314188413885</v>
+        <v>0.9711314188413888</v>
       </c>
       <c r="F8">
-        <v>0.9348126731630805</v>
+        <v>0.9348126731630808</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -667,16 +667,16 @@
         <v>1.031750818426121</v>
       </c>
       <c r="J8">
-        <v>0.9854127901065353</v>
+        <v>0.9854127901065356</v>
       </c>
       <c r="K8">
         <v>1.000087117794564</v>
       </c>
       <c r="L8">
-        <v>0.9827171729055607</v>
+        <v>0.9827171729055609</v>
       </c>
       <c r="M8">
-        <v>0.9469545705595352</v>
+        <v>0.9469545705595354</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -687,16 +687,16 @@
         <v>1.05</v>
       </c>
       <c r="C9">
-        <v>0.9316311116654397</v>
+        <v>0.9316311116654393</v>
       </c>
       <c r="D9">
-        <v>0.9648553013414848</v>
+        <v>0.9648553013414847</v>
       </c>
       <c r="E9">
-        <v>0.9441492316796402</v>
+        <v>0.9441492316796399</v>
       </c>
       <c r="F9">
-        <v>0.8942193455640146</v>
+        <v>0.8942193455640142</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -705,16 +705,16 @@
         <v>1.021057184722024</v>
       </c>
       <c r="J9">
-        <v>0.9598527595003981</v>
+        <v>0.9598527595003979</v>
       </c>
       <c r="K9">
-        <v>0.9785455307592807</v>
+        <v>0.9785455307592804</v>
       </c>
       <c r="L9">
         <v>0.9582184718385207</v>
       </c>
       <c r="M9">
-        <v>0.9092984532138478</v>
+        <v>0.9092984532138475</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -725,16 +725,16 @@
         <v>1.05</v>
       </c>
       <c r="C10">
-        <v>0.907397701900307</v>
+        <v>0.9073977019003059</v>
       </c>
       <c r="D10">
-        <v>0.9462640807014276</v>
+        <v>0.946264080701427</v>
       </c>
       <c r="E10">
-        <v>0.923118321145717</v>
+        <v>0.9231183211457161</v>
       </c>
       <c r="F10">
-        <v>0.8621588305499388</v>
+        <v>0.8621588305499376</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -743,16 +743,16 @@
         <v>1.012587897571456</v>
       </c>
       <c r="J10">
-        <v>0.9398365673058284</v>
+        <v>0.9398365673058273</v>
       </c>
       <c r="K10">
-        <v>0.9616764151829899</v>
+        <v>0.9616764151829891</v>
       </c>
       <c r="L10">
-        <v>0.9390298109139052</v>
+        <v>0.9390298109139041</v>
       </c>
       <c r="M10">
-        <v>0.8795597137628783</v>
+        <v>0.879559713762877</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -763,16 +763,16 @@
         <v>1.05</v>
       </c>
       <c r="C11">
-        <v>0.8956943323388814</v>
+        <v>0.8956943323388811</v>
       </c>
       <c r="D11">
-        <v>0.9373131531172861</v>
+        <v>0.9373131531172858</v>
       </c>
       <c r="E11">
-        <v>0.9129780194690182</v>
+        <v>0.9129780194690177</v>
       </c>
       <c r="F11">
-        <v>0.8465235088581691</v>
+        <v>0.8465235088581685</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -781,16 +781,16 @@
         <v>1.008472014280511</v>
       </c>
       <c r="J11">
-        <v>0.9301568154135416</v>
+        <v>0.9301568154135413</v>
       </c>
       <c r="K11">
-        <v>0.9535226828955768</v>
+        <v>0.9535226828955764</v>
       </c>
       <c r="L11">
-        <v>0.929751460199819</v>
+        <v>0.9297514601998186</v>
       </c>
       <c r="M11">
-        <v>0.8650645461225331</v>
+        <v>0.8650645461225328</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -801,16 +801,16 @@
         <v>1.05</v>
       </c>
       <c r="C12">
-        <v>0.8911172841029515</v>
+        <v>0.891117284102951</v>
       </c>
       <c r="D12">
-        <v>0.9338179598209763</v>
+        <v>0.9338179598209759</v>
       </c>
       <c r="E12">
-        <v>0.9090155814828322</v>
+        <v>0.9090155814828318</v>
       </c>
       <c r="F12">
-        <v>0.8403770291737926</v>
+        <v>0.8403770291737916</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -819,16 +819,16 @@
         <v>1.006858792069812</v>
       </c>
       <c r="J12">
-        <v>0.9263692143795209</v>
+        <v>0.9263692143795201</v>
       </c>
       <c r="K12">
-        <v>0.9503333119458934</v>
+        <v>0.9503333119458929</v>
       </c>
       <c r="L12">
-        <v>0.9261213977907007</v>
+        <v>0.9261213977907001</v>
       </c>
       <c r="M12">
-        <v>0.8593684718465312</v>
+        <v>0.8593684718465303</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -839,34 +839,34 @@
         <v>1.05</v>
       </c>
       <c r="C13">
-        <v>0.8921104809512194</v>
+        <v>0.8921104809512223</v>
       </c>
       <c r="D13">
-        <v>0.9345761322968363</v>
+        <v>0.9345761322968389</v>
       </c>
       <c r="E13">
-        <v>0.9098752456042147</v>
+        <v>0.9098752456042174</v>
       </c>
       <c r="F13">
-        <v>0.8417123933540499</v>
+        <v>0.8417123933540531</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="I13">
-        <v>1.007209006647755</v>
+        <v>1.007209006647757</v>
       </c>
       <c r="J13">
-        <v>0.9271911939522602</v>
+        <v>0.9271911939522631</v>
       </c>
       <c r="K13">
-        <v>0.9510254047812802</v>
+        <v>0.9510254047812826</v>
       </c>
       <c r="L13">
-        <v>0.9269091610735593</v>
+        <v>0.9269091610735616</v>
       </c>
       <c r="M13">
-        <v>0.860605862776388</v>
+        <v>0.860605862776391</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -877,34 +877,34 @@
         <v>1.05</v>
       </c>
       <c r="C14">
-        <v>0.8953210341157214</v>
+        <v>0.8953210341157238</v>
       </c>
       <c r="D14">
-        <v>0.937027972615743</v>
+        <v>0.9370279726157449</v>
       </c>
       <c r="E14">
-        <v>0.9126547758349005</v>
+        <v>0.9126547758349024</v>
       </c>
       <c r="F14">
-        <v>0.8460229098850993</v>
+        <v>0.8460229098851015</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>1.008340510983428</v>
+        <v>1.008340510983429</v>
       </c>
       <c r="J14">
-        <v>0.9298479431062286</v>
+        <v>0.9298479431062309</v>
       </c>
       <c r="K14">
-        <v>0.9532625694901026</v>
+        <v>0.9532625694901045</v>
       </c>
       <c r="L14">
-        <v>0.9294554232320059</v>
+        <v>0.9294554232320075</v>
       </c>
       <c r="M14">
-        <v>0.8646005790482725</v>
+        <v>0.8646005790482746</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -915,34 +915,34 @@
         <v>1.05</v>
       </c>
       <c r="C15">
-        <v>0.8972669140676258</v>
+        <v>0.8972669140676232</v>
       </c>
       <c r="D15">
-        <v>0.9385147491678759</v>
+        <v>0.9385147491678737</v>
       </c>
       <c r="E15">
-        <v>0.9143398762245681</v>
+        <v>0.9143398762245655</v>
       </c>
       <c r="F15">
-        <v>0.8486310345940273</v>
+        <v>0.8486310345940241</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="I15">
-        <v>1.009025853947287</v>
+        <v>1.009025853947286</v>
       </c>
       <c r="J15">
-        <v>0.9314579132077556</v>
+        <v>0.9314579132077532</v>
       </c>
       <c r="K15">
-        <v>0.9546184359417142</v>
+        <v>0.9546184359417119</v>
       </c>
       <c r="L15">
-        <v>0.9309985112898104</v>
+        <v>0.930998511289808</v>
       </c>
       <c r="M15">
-        <v>0.8670179460468076</v>
+        <v>0.8670179460468045</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -953,16 +953,16 @@
         <v>1.05</v>
       </c>
       <c r="C16">
-        <v>0.9081452452064335</v>
+        <v>0.9081452452064337</v>
       </c>
       <c r="D16">
-        <v>0.9468364630148371</v>
+        <v>0.9468364630148374</v>
       </c>
       <c r="E16">
-        <v>0.9237664178091097</v>
+        <v>0.9237664178091098</v>
       </c>
       <c r="F16">
-        <v>0.8631538301876132</v>
+        <v>0.8631538301876135</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -977,10 +977,10 @@
         <v>0.962197127173004</v>
       </c>
       <c r="L16">
-        <v>0.9396222526095704</v>
+        <v>0.9396222526095708</v>
       </c>
       <c r="M16">
-        <v>0.8804823864989494</v>
+        <v>0.8804823864989497</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -991,16 +991,16 @@
         <v>1.05</v>
       </c>
       <c r="C17">
-        <v>0.9146165996200242</v>
+        <v>0.9146165996200245</v>
       </c>
       <c r="D17">
-        <v>0.9517945839507459</v>
+        <v>0.9517945839507462</v>
       </c>
       <c r="E17">
         <v>0.9293787354729477</v>
       </c>
       <c r="F17">
-        <v>0.8717502251078336</v>
+        <v>0.8717502251078343</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1009,16 +1009,16 @@
         <v>1.015119142697466</v>
       </c>
       <c r="J17">
-        <v>0.9458033114859983</v>
+        <v>0.9458033114859984</v>
       </c>
       <c r="K17">
-        <v>0.9667041358556328</v>
+        <v>0.9667041358556331</v>
       </c>
       <c r="L17">
-        <v>0.9447497140589678</v>
+        <v>0.944749714058968</v>
       </c>
       <c r="M17">
-        <v>0.888454828057236</v>
+        <v>0.8884548280572365</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1029,34 +1029,34 @@
         <v>1.05</v>
       </c>
       <c r="C18">
-        <v>0.9182784836108141</v>
+        <v>0.9182784836108171</v>
       </c>
       <c r="D18">
-        <v>0.9546025835734198</v>
+        <v>0.954602583573422</v>
       </c>
       <c r="E18">
-        <v>0.9325559445006</v>
+        <v>0.9325559445006029</v>
       </c>
       <c r="F18">
-        <v>0.87660157059847</v>
+        <v>0.8766015705984733</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="I18">
-        <v>1.016400650230964</v>
+        <v>1.016400650230966</v>
       </c>
       <c r="J18">
-        <v>0.9488287648231966</v>
+        <v>0.9488287648231993</v>
       </c>
       <c r="K18">
-        <v>0.9692538167337013</v>
+        <v>0.9692538167337035</v>
       </c>
       <c r="L18">
-        <v>0.9476501012508087</v>
+        <v>0.9476501012508116</v>
       </c>
       <c r="M18">
-        <v>0.8929546753365882</v>
+        <v>0.8929546753365916</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1067,16 +1067,16 @@
         <v>1.05</v>
       </c>
       <c r="C19">
-        <v>0.9195091344571956</v>
+        <v>0.9195091344571954</v>
       </c>
       <c r="D19">
-        <v>0.9555466453416136</v>
+        <v>0.9555466453416134</v>
       </c>
       <c r="E19">
-        <v>0.9336239316254485</v>
+        <v>0.9336239316254484</v>
       </c>
       <c r="F19">
-        <v>0.8782299522448411</v>
+        <v>0.8782299522448412</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1085,13 +1085,13 @@
         <v>1.016830922557188</v>
       </c>
       <c r="J19">
-        <v>0.9498453300705116</v>
+        <v>0.9498453300705115</v>
       </c>
       <c r="K19">
-        <v>0.970110565379452</v>
+        <v>0.9701105653794517</v>
       </c>
       <c r="L19">
-        <v>0.9486246520406572</v>
+        <v>0.9486246520406569</v>
       </c>
       <c r="M19">
         <v>0.8944651589477618</v>
@@ -1105,16 +1105,16 @@
         <v>1.05</v>
       </c>
       <c r="C20">
-        <v>0.9139342339186914</v>
+        <v>0.9139342339186912</v>
       </c>
       <c r="D20">
-        <v>0.9512715216781357</v>
+        <v>0.9512715216781354</v>
       </c>
       <c r="E20">
-        <v>0.9287867965955299</v>
+        <v>0.9287867965955293</v>
       </c>
       <c r="F20">
-        <v>0.8708451974178761</v>
+        <v>0.8708451974178762</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1123,13 +1123,13 @@
         <v>1.014880149997224</v>
       </c>
       <c r="J20">
-        <v>0.9452394438435265</v>
+        <v>0.9452394438435262</v>
       </c>
       <c r="K20">
-        <v>0.966228964483682</v>
+        <v>0.9662289644836818</v>
       </c>
       <c r="L20">
-        <v>0.9442091610324973</v>
+        <v>0.944209161032497</v>
       </c>
       <c r="M20">
         <v>0.8876154188219648</v>
@@ -1140,19 +1140,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1.05</v>
+        <v>1.049999999999999</v>
       </c>
       <c r="C21">
-        <v>0.8943824422579156</v>
+        <v>0.8943824422579176</v>
       </c>
       <c r="D21">
-        <v>0.9363110282145427</v>
+        <v>0.9363110282145444</v>
       </c>
       <c r="E21">
-        <v>0.9118420934833724</v>
+        <v>0.911842093483374</v>
       </c>
       <c r="F21">
-        <v>0.8447637008236291</v>
+        <v>0.8447637008236313</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1161,16 +1161,16 @@
         <v>1.008009814029496</v>
       </c>
       <c r="J21">
-        <v>0.9290713073058597</v>
+        <v>0.9290713073058616</v>
       </c>
       <c r="K21">
-        <v>0.952608553923681</v>
+        <v>0.9526085539236827</v>
       </c>
       <c r="L21">
-        <v>0.9287110697000825</v>
+        <v>0.9287110697000841</v>
       </c>
       <c r="M21">
-        <v>0.8634335531885015</v>
+        <v>0.8634335531885033</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1181,34 +1181,34 @@
         <v>1.05</v>
       </c>
       <c r="C22">
-        <v>0.880717593945458</v>
+        <v>0.8807175939454568</v>
       </c>
       <c r="D22">
-        <v>0.9258883659122696</v>
+        <v>0.9258883659122688</v>
       </c>
       <c r="E22">
-        <v>0.9000198350212724</v>
+        <v>0.9000198350212716</v>
       </c>
       <c r="F22">
-        <v>0.8263376754712235</v>
+        <v>0.8263376754712221</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>1.003187109790833</v>
+        <v>1.003187109790832</v>
       </c>
       <c r="J22">
-        <v>0.9177595056695752</v>
+        <v>0.9177595056695742</v>
       </c>
       <c r="K22">
-        <v>0.9430862826721248</v>
+        <v>0.943086282672124</v>
       </c>
       <c r="L22">
-        <v>0.9178711619770821</v>
+        <v>0.9178711619770813</v>
       </c>
       <c r="M22">
-        <v>0.8463636624432069</v>
+        <v>0.8463636624432055</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1219,16 +1219,16 @@
         <v>1.05</v>
       </c>
       <c r="C23">
-        <v>0.8881138298323769</v>
+        <v>0.888113829832376</v>
       </c>
       <c r="D23">
-        <v>0.9315261411962814</v>
+        <v>0.9315261411962809</v>
       </c>
       <c r="E23">
-        <v>0.9064165031559047</v>
+        <v>0.9064165031559037</v>
       </c>
       <c r="F23">
-        <v>0.8363332608366524</v>
+        <v>0.8363332608366504</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1237,16 +1237,16 @@
         <v>1.005799242324163</v>
       </c>
       <c r="J23">
-        <v>0.9238832334969861</v>
+        <v>0.9238832334969853</v>
       </c>
       <c r="K23">
-        <v>0.9482403705775079</v>
+        <v>0.9482403705775073</v>
       </c>
       <c r="L23">
-        <v>0.9237390010982309</v>
+        <v>0.9237390010982299</v>
       </c>
       <c r="M23">
-        <v>0.8556218169788331</v>
+        <v>0.8556218169788312</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1257,13 +1257,13 @@
         <v>1.05</v>
       </c>
       <c r="C24">
-        <v>0.9142429106618803</v>
+        <v>0.9142429106618798</v>
       </c>
       <c r="D24">
-        <v>0.9515081280947616</v>
+        <v>0.9515081280947608</v>
       </c>
       <c r="E24">
-        <v>0.9290545632355585</v>
+        <v>0.9290545632355581</v>
       </c>
       <c r="F24">
         <v>0.8712546382745128</v>
@@ -1275,13 +1275,13 @@
         <v>1.014988268704023</v>
       </c>
       <c r="J24">
-        <v>0.9454945201734463</v>
+        <v>0.9454945201734462</v>
       </c>
       <c r="K24">
-        <v>0.9664439163461324</v>
+        <v>0.9664439163461319</v>
       </c>
       <c r="L24">
-        <v>0.9444536902977833</v>
+        <v>0.944453690297783</v>
       </c>
       <c r="M24">
         <v>0.8879951715297911</v>
@@ -1295,16 +1295,16 @@
         <v>1.05</v>
       </c>
       <c r="C25">
-        <v>0.9401828664177465</v>
+        <v>0.9401828664177455</v>
       </c>
       <c r="D25">
-        <v>0.9714320536376383</v>
+        <v>0.9714320536376375</v>
       </c>
       <c r="E25">
-        <v>0.9515801131224424</v>
+        <v>0.9515801131224416</v>
       </c>
       <c r="F25">
-        <v>0.9054497260859371</v>
+        <v>0.9054497260859358</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1313,16 +1313,16 @@
         <v>1.024024040950465</v>
       </c>
       <c r="J25">
-        <v>0.9669057788575415</v>
+        <v>0.9669057788575406</v>
       </c>
       <c r="K25">
-        <v>0.9844906534933383</v>
+        <v>0.9844906534933375</v>
       </c>
       <c r="L25">
-        <v>0.9649796653326759</v>
+        <v>0.964979665332675</v>
       </c>
       <c r="M25">
-        <v>0.9197175616023169</v>
+        <v>0.9197175616023154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>